<commit_message>
#11 - Fix dict, df and search bugs
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -480,7 +480,7 @@
         <v>1404.55</v>
       </c>
       <c r="D2">
-        <v>2995.05</v>
+        <v>2998.05</v>
       </c>
       <c r="E2">
         <v>2388.84</v>
@@ -497,7 +497,7 @@
         <v>194.79</v>
       </c>
       <c r="D3">
-        <v>307.14</v>
+        <v>402.89</v>
       </c>
       <c r="E3">
         <v>1313.862</v>
@@ -514,7 +514,7 @@
         <v>90.52</v>
       </c>
       <c r="D4">
-        <v>99.88</v>
+        <v>36.28</v>
       </c>
       <c r="E4">
         <v>358.326</v>
@@ -531,7 +531,7 @@
         <v>35.89</v>
       </c>
       <c r="D5">
-        <v>162.15</v>
+        <v>149.21</v>
       </c>
       <c r="E5">
         <v>716.652</v>
@@ -548,7 +548,7 @@
         <v>29.47</v>
       </c>
       <c r="D6">
-        <v>46.02</v>
+        <v>50.74</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -565,7 +565,7 @@
         <v>122.22</v>
       </c>
       <c r="D7">
-        <v>253.77</v>
+        <v>137.51</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -582,7 +582,7 @@
         <v>219.6</v>
       </c>
       <c r="D8">
-        <v>869.36</v>
+        <v>858.8099999999999</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -599,7 +599,7 @@
         <v>2623.22</v>
       </c>
       <c r="D9">
-        <v>1961.59</v>
+        <v>918.87</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>2241.43</v>
       </c>
       <c r="D10">
-        <v>3511.2</v>
+        <v>3513.91</v>
       </c>
       <c r="E10">
         <v>3510</v>
@@ -633,7 +633,7 @@
         <v>13.55</v>
       </c>
       <c r="D11">
-        <v>20.83</v>
+        <v>17.24</v>
       </c>
       <c r="E11">
         <v>6.8</v>
@@ -650,7 +650,7 @@
         <v>309.36</v>
       </c>
       <c r="D12">
-        <v>425.54</v>
+        <v>371.54</v>
       </c>
       <c r="E12">
         <v>303</v>
@@ -667,7 +667,7 @@
         <v>0.7</v>
       </c>
       <c r="D13">
-        <v>1.52</v>
+        <v>0.64</v>
       </c>
       <c r="E13">
         <v>0.9</v>
@@ -684,7 +684,7 @@
         <v>0.95</v>
       </c>
       <c r="D14">
-        <v>1.16</v>
+        <v>0.68</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>11.74</v>
       </c>
       <c r="D15">
-        <v>11.65</v>
+        <v>3.53</v>
       </c>
       <c r="E15">
         <v>11.5</v>
@@ -718,7 +718,7 @@
         <v>0.52</v>
       </c>
       <c r="D16">
-        <v>0.52</v>
+        <v>0.89</v>
       </c>
       <c r="E16">
         <v>1.1</v>
@@ -735,7 +735,7 @@
         <v>4.06</v>
       </c>
       <c r="D17">
-        <v>4.75</v>
+        <v>0.75</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -752,7 +752,7 @@
         <v>3.74</v>
       </c>
       <c r="D18">
-        <v>95.5</v>
+        <v>52.68</v>
       </c>
       <c r="E18">
         <v>66.09999999999999</v>
@@ -769,7 +769,7 @@
         <v>41.23</v>
       </c>
       <c r="D19">
-        <v>565.72</v>
+        <v>561.75</v>
       </c>
       <c r="E19">
         <v>560</v>
@@ -786,7 +786,7 @@
         <v>1.39</v>
       </c>
       <c r="D20">
-        <v>2.43</v>
+        <v>2.12</v>
       </c>
       <c r="E20">
         <v>0.7</v>
@@ -803,7 +803,7 @@
         <v>481.27</v>
       </c>
       <c r="D21">
-        <v>321.66</v>
+        <v>329.46</v>
       </c>
       <c r="E21">
         <v>322</v>
@@ -820,7 +820,7 @@
         <v>989.78</v>
       </c>
       <c r="D22">
-        <v>1054.93</v>
+        <v>650.91</v>
       </c>
       <c r="E22">
         <v>8</v>
@@ -837,7 +837,7 @@
         <v>16.71</v>
       </c>
       <c r="D23">
-        <v>16.81</v>
+        <v>5.05</v>
       </c>
       <c r="E23">
         <v>649</v>

</xml_diff>

<commit_message>
#47 Fix nutrition list and quantities
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -480,7 +480,7 @@
         <v>1404.55</v>
       </c>
       <c r="D2">
-        <v>2998.05</v>
+        <v>3002.05</v>
       </c>
       <c r="E2">
         <v>2388.84</v>
@@ -497,7 +497,7 @@
         <v>194.79</v>
       </c>
       <c r="D3">
-        <v>402.89</v>
+        <v>428.3</v>
       </c>
       <c r="E3">
         <v>1313.862</v>
@@ -514,7 +514,7 @@
         <v>90.52</v>
       </c>
       <c r="D4">
-        <v>36.28</v>
+        <v>60.56</v>
       </c>
       <c r="E4">
         <v>358.326</v>
@@ -531,7 +531,7 @@
         <v>35.89</v>
       </c>
       <c r="D5">
-        <v>149.21</v>
+        <v>123.43</v>
       </c>
       <c r="E5">
         <v>716.652</v>
@@ -548,7 +548,7 @@
         <v>29.47</v>
       </c>
       <c r="D6">
-        <v>50.74</v>
+        <v>32.08</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -565,7 +565,7 @@
         <v>122.22</v>
       </c>
       <c r="D7">
-        <v>137.51</v>
+        <v>125.12</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -582,7 +582,7 @@
         <v>219.6</v>
       </c>
       <c r="D8">
-        <v>858.8099999999999</v>
+        <v>862.29</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -599,7 +599,7 @@
         <v>2623.22</v>
       </c>
       <c r="D9">
-        <v>918.87</v>
+        <v>1213.84</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>2241.43</v>
       </c>
       <c r="D10">
-        <v>3513.91</v>
+        <v>3509.07</v>
       </c>
       <c r="E10">
         <v>3510</v>
@@ -633,7 +633,7 @@
         <v>13.55</v>
       </c>
       <c r="D11">
-        <v>17.24</v>
+        <v>11.77</v>
       </c>
       <c r="E11">
         <v>6.8</v>
@@ -650,7 +650,7 @@
         <v>309.36</v>
       </c>
       <c r="D12">
-        <v>371.54</v>
+        <v>406.49</v>
       </c>
       <c r="E12">
         <v>303</v>
@@ -667,7 +667,7 @@
         <v>0.7</v>
       </c>
       <c r="D13">
-        <v>0.64</v>
+        <v>0.8</v>
       </c>
       <c r="E13">
         <v>0.9</v>
@@ -684,7 +684,7 @@
         <v>0.95</v>
       </c>
       <c r="D14">
-        <v>0.68</v>
+        <v>0.83</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>11.74</v>
       </c>
       <c r="D15">
-        <v>3.53</v>
+        <v>14.72</v>
       </c>
       <c r="E15">
         <v>11.5</v>
@@ -718,7 +718,7 @@
         <v>0.52</v>
       </c>
       <c r="D16">
-        <v>0.89</v>
+        <v>1.39</v>
       </c>
       <c r="E16">
         <v>1.1</v>
@@ -735,7 +735,7 @@
         <v>4.06</v>
       </c>
       <c r="D17">
-        <v>0.75</v>
+        <v>2.19</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -752,7 +752,7 @@
         <v>3.74</v>
       </c>
       <c r="D18">
-        <v>52.68</v>
+        <v>70.31</v>
       </c>
       <c r="E18">
         <v>66.09999999999999</v>
@@ -769,7 +769,7 @@
         <v>41.23</v>
       </c>
       <c r="D19">
-        <v>561.75</v>
+        <v>563.7</v>
       </c>
       <c r="E19">
         <v>560</v>
@@ -786,7 +786,7 @@
         <v>1.39</v>
       </c>
       <c r="D20">
-        <v>2.12</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>0.7</v>
@@ -803,7 +803,7 @@
         <v>481.27</v>
       </c>
       <c r="D21">
-        <v>329.46</v>
+        <v>298.14</v>
       </c>
       <c r="E21">
         <v>322</v>
@@ -820,7 +820,7 @@
         <v>989.78</v>
       </c>
       <c r="D22">
-        <v>650.91</v>
+        <v>650.89</v>
       </c>
       <c r="E22">
         <v>8</v>
@@ -837,7 +837,7 @@
         <v>16.71</v>
       </c>
       <c r="D23">
-        <v>5.05</v>
+        <v>6.21</v>
       </c>
       <c r="E23">
         <v>649</v>

</xml_diff>

<commit_message>
#44 Fix step that not empty the food quantity
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Nutrient</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>FIBRA</t>
+  </si>
+  <si>
+    <t>AGPOLI</t>
+  </si>
+  <si>
+    <t>AGTRANS</t>
+  </si>
+  <si>
+    <t>AGSAT</t>
   </si>
   <si>
     <t>COLEST</t>
@@ -449,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,7 +489,7 @@
         <v>1404.55</v>
       </c>
       <c r="D2">
-        <v>3002.05</v>
+        <v>502.35</v>
       </c>
       <c r="E2">
         <v>2388.84</v>
@@ -497,7 +506,7 @@
         <v>194.79</v>
       </c>
       <c r="D3">
-        <v>428.3</v>
+        <v>96.88</v>
       </c>
       <c r="E3">
         <v>1313.862</v>
@@ -514,10 +523,10 @@
         <v>90.52</v>
       </c>
       <c r="D4">
-        <v>60.56</v>
+        <v>24.12</v>
       </c>
       <c r="E4">
-        <v>358.326</v>
+        <v>238.884</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -531,10 +540,10 @@
         <v>35.89</v>
       </c>
       <c r="D5">
-        <v>123.43</v>
+        <v>7.64</v>
       </c>
       <c r="E5">
-        <v>716.652</v>
+        <v>358.326</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -548,7 +557,7 @@
         <v>29.47</v>
       </c>
       <c r="D6">
-        <v>32.08</v>
+        <v>25.26</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -562,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>122.22</v>
+        <v>11.47</v>
       </c>
       <c r="D7">
-        <v>125.12</v>
+        <v>3.87</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -579,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>219.6</v>
+        <v>0.9</v>
       </c>
       <c r="D8">
-        <v>862.29</v>
+        <v>0.17</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -596,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>2623.22</v>
+        <v>11.01</v>
       </c>
       <c r="D9">
-        <v>1213.84</v>
+        <v>1.53</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>23.8884</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -613,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>2241.43</v>
+        <v>122.22</v>
       </c>
       <c r="D10">
-        <v>3509.07</v>
+        <v>5.38</v>
       </c>
       <c r="E10">
-        <v>3510</v>
+        <v>238.884</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -630,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>13.55</v>
+        <v>219.6</v>
       </c>
       <c r="D11">
-        <v>11.77</v>
+        <v>107.01</v>
       </c>
       <c r="E11">
-        <v>6.8</v>
+        <v>143.3304</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -647,13 +656,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>309.36</v>
+        <v>2623.22</v>
       </c>
       <c r="D12">
-        <v>406.49</v>
+        <v>1047.94</v>
       </c>
       <c r="E12">
-        <v>303</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -664,13 +673,13 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0.7</v>
+        <v>2241.43</v>
       </c>
       <c r="D13">
-        <v>0.8</v>
+        <v>1085.02</v>
       </c>
       <c r="E13">
-        <v>0.9</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -681,13 +690,13 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0.95</v>
+        <v>13.55</v>
       </c>
       <c r="D14">
-        <v>0.83</v>
+        <v>7.1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -698,13 +707,13 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>11.74</v>
+        <v>309.36</v>
       </c>
       <c r="D15">
-        <v>14.72</v>
+        <v>170.19</v>
       </c>
       <c r="E15">
-        <v>11.5</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -715,13 +724,13 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="D16">
-        <v>1.39</v>
+        <v>0.36</v>
       </c>
       <c r="E16">
-        <v>1.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -732,13 +741,13 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>4.06</v>
+        <v>0.95</v>
       </c>
       <c r="D17">
-        <v>2.19</v>
+        <v>0.36</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -749,13 +758,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>3.74</v>
+        <v>11.74</v>
       </c>
       <c r="D18">
-        <v>70.31</v>
+        <v>1.65</v>
       </c>
       <c r="E18">
-        <v>66.09999999999999</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -766,13 +775,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>41.23</v>
+        <v>0.52</v>
       </c>
       <c r="D19">
-        <v>563.7</v>
+        <v>0.35</v>
       </c>
       <c r="E19">
-        <v>560</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -783,13 +792,13 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1.39</v>
+        <v>4.06</v>
       </c>
       <c r="D20">
+        <v>0.18</v>
+      </c>
+      <c r="E20">
         <v>2</v>
-      </c>
-      <c r="E20">
-        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -800,13 +809,13 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>481.27</v>
+        <v>3.74</v>
       </c>
       <c r="D21">
-        <v>298.14</v>
+        <v>1.62</v>
       </c>
       <c r="E21">
-        <v>322</v>
+        <v>66.09999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -817,13 +826,13 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>989.78</v>
+        <v>41.23</v>
       </c>
       <c r="D22">
-        <v>650.89</v>
+        <v>1.61</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>560</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -834,12 +843,63 @@
         <v>25</v>
       </c>
       <c r="C23">
+        <v>1.39</v>
+      </c>
+      <c r="D23">
+        <v>0.78</v>
+      </c>
+      <c r="E23">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>481.27</v>
+      </c>
+      <c r="D24">
+        <v>406.45</v>
+      </c>
+      <c r="E24">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>989.78</v>
+      </c>
+      <c r="D25">
+        <v>396.61</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
         <v>16.71</v>
       </c>
-      <c r="D23">
-        <v>6.21</v>
-      </c>
-      <c r="E23">
+      <c r="D26">
+        <v>3.57</v>
+      </c>
+      <c r="E26">
         <v>649</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#55 #47  Fix nutrients order and improve papaSearch heuristic
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -43,21 +43,21 @@
     <t>FIBRA</t>
   </si>
   <si>
+    <t>COLEST</t>
+  </si>
+  <si>
+    <t>CALCIO</t>
+  </si>
+  <si>
+    <t>AGTRANS</t>
+  </si>
+  <si>
+    <t>AGSAT</t>
+  </si>
+  <si>
     <t>AGPOLI</t>
   </si>
   <si>
-    <t>AGTRANS</t>
-  </si>
-  <si>
-    <t>AGSAT</t>
-  </si>
-  <si>
-    <t>COLEST</t>
-  </si>
-  <si>
-    <t>CALCIO</t>
-  </si>
-  <si>
     <t>SODIO</t>
   </si>
   <si>
@@ -76,10 +76,10 @@
     <t>RIBOFLAVINA</t>
   </si>
   <si>
+    <t>PIRIDOXAMINA</t>
+  </si>
+  <si>
     <t>NIACINA</t>
-  </si>
-  <si>
-    <t>PIRIDOXAMINA</t>
   </si>
   <si>
     <t>COBALAMINA</t>
@@ -489,10 +489,10 @@
         <v>1404.55</v>
       </c>
       <c r="D2">
-        <v>502.35</v>
+        <v>4332.95</v>
       </c>
       <c r="E2">
-        <v>2388.84</v>
+        <v>2989.87</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -506,10 +506,10 @@
         <v>194.79</v>
       </c>
       <c r="D3">
-        <v>96.88</v>
+        <v>805.3</v>
       </c>
       <c r="E3">
-        <v>1313.862</v>
+        <v>1644.4285</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -523,10 +523,10 @@
         <v>90.52</v>
       </c>
       <c r="D4">
-        <v>24.12</v>
+        <v>111.79</v>
       </c>
       <c r="E4">
-        <v>238.884</v>
+        <v>298.987</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -540,10 +540,10 @@
         <v>35.89</v>
       </c>
       <c r="D5">
-        <v>7.64</v>
+        <v>81.73999999999999</v>
       </c>
       <c r="E5">
-        <v>358.326</v>
+        <v>448.4805000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -557,7 +557,7 @@
         <v>29.47</v>
       </c>
       <c r="D6">
-        <v>25.26</v>
+        <v>34.27</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>11.47</v>
+        <v>122.22</v>
       </c>
       <c r="D7">
-        <v>3.87</v>
+        <v>261.75</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0.9</v>
+        <v>219.6</v>
       </c>
       <c r="D8">
-        <v>0.17</v>
+        <v>720</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>11.01</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
-        <v>1.53</v>
+        <v>1.25</v>
       </c>
       <c r="E9">
-        <v>23.8884</v>
+        <v>29.89870000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>122.22</v>
+        <v>11.01</v>
       </c>
       <c r="D10">
-        <v>5.38</v>
+        <v>29.47</v>
       </c>
       <c r="E10">
-        <v>238.884</v>
+        <v>298.987</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>219.6</v>
+        <v>11.47</v>
       </c>
       <c r="D11">
-        <v>107.01</v>
+        <v>20.61</v>
       </c>
       <c r="E11">
-        <v>143.3304</v>
+        <v>179.3922</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -659,7 +659,7 @@
         <v>2623.22</v>
       </c>
       <c r="D12">
-        <v>1047.94</v>
+        <v>3059.56</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -676,7 +676,7 @@
         <v>2241.43</v>
       </c>
       <c r="D13">
-        <v>1085.02</v>
+        <v>3721.76</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -693,7 +693,7 @@
         <v>13.55</v>
       </c>
       <c r="D14">
-        <v>7.1</v>
+        <v>17.37</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -710,7 +710,7 @@
         <v>309.36</v>
       </c>
       <c r="D15">
-        <v>170.19</v>
+        <v>326.25</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -727,7 +727,7 @@
         <v>0.7</v>
       </c>
       <c r="D16">
-        <v>0.36</v>
+        <v>1.2</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -744,7 +744,7 @@
         <v>0.95</v>
       </c>
       <c r="D17">
-        <v>0.36</v>
+        <v>2.15</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,13 +758,13 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>11.74</v>
+        <v>0.52</v>
       </c>
       <c r="D18">
-        <v>1.65</v>
+        <v>0.96</v>
       </c>
       <c r="E18">
-        <v>11.5</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -775,13 +775,13 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>0.52</v>
+        <v>11.74</v>
       </c>
       <c r="D19">
-        <v>0.35</v>
+        <v>16.52</v>
       </c>
       <c r="E19">
-        <v>1.1</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -795,7 +795,7 @@
         <v>4.06</v>
       </c>
       <c r="D20">
-        <v>0.18</v>
+        <v>5.76</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -812,7 +812,7 @@
         <v>3.74</v>
       </c>
       <c r="D21">
-        <v>1.62</v>
+        <v>51.94</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -829,7 +829,7 @@
         <v>41.23</v>
       </c>
       <c r="D22">
-        <v>1.61</v>
+        <v>661.71</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -846,7 +846,7 @@
         <v>1.39</v>
       </c>
       <c r="D23">
-        <v>0.78</v>
+        <v>1.56</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -863,7 +863,7 @@
         <v>481.27</v>
       </c>
       <c r="D24">
-        <v>406.45</v>
+        <v>552.47</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -880,10 +880,10 @@
         <v>989.78</v>
       </c>
       <c r="D25">
-        <v>396.61</v>
+        <v>1406.34</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>649</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -897,10 +897,10 @@
         <v>16.71</v>
       </c>
       <c r="D26">
-        <v>3.57</v>
+        <v>19.54</v>
       </c>
       <c r="E26">
-        <v>649</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#60 Add preselect option by strata
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1404.55</v>
+        <v>1307.95</v>
       </c>
       <c r="D2">
-        <v>4332.95</v>
+        <v>4638.95</v>
       </c>
       <c r="E2">
-        <v>2989.87</v>
+        <v>1765.61</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>194.79</v>
+        <v>206.19</v>
       </c>
       <c r="D3">
-        <v>805.3</v>
+        <v>697.52</v>
       </c>
       <c r="E3">
-        <v>1644.4285</v>
+        <v>971.0855</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>90.52</v>
+        <v>42.31</v>
       </c>
       <c r="D4">
-        <v>111.79</v>
+        <v>162.59</v>
       </c>
       <c r="E4">
-        <v>298.987</v>
+        <v>176.561</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>35.89</v>
+        <v>40.18</v>
       </c>
       <c r="D5">
-        <v>81.73999999999999</v>
+        <v>144.5</v>
       </c>
       <c r="E5">
-        <v>448.4805000000001</v>
+        <v>264.8415</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>29.47</v>
+        <v>23.37</v>
       </c>
       <c r="D6">
-        <v>34.27</v>
+        <v>52.49</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>122.22</v>
+        <v>46.93</v>
       </c>
       <c r="D7">
-        <v>261.75</v>
+        <v>773.48</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>219.6</v>
+        <v>199.15</v>
       </c>
       <c r="D8">
-        <v>720</v>
+        <v>536.14</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="D9">
-        <v>1.25</v>
+        <v>1.17</v>
       </c>
       <c r="E9">
-        <v>29.89870000000001</v>
+        <v>17.6561</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>11.01</v>
+        <v>11.46</v>
       </c>
       <c r="D10">
-        <v>29.47</v>
+        <v>49.11</v>
       </c>
       <c r="E10">
-        <v>298.987</v>
+        <v>176.561</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>11.47</v>
+        <v>7.2</v>
       </c>
       <c r="D11">
-        <v>20.61</v>
+        <v>32.98</v>
       </c>
       <c r="E11">
-        <v>179.3922</v>
+        <v>105.9366</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2623.22</v>
+        <v>1411.22</v>
       </c>
       <c r="D12">
-        <v>3059.56</v>
+        <v>2808.04</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2241.43</v>
+        <v>1418.91</v>
       </c>
       <c r="D13">
-        <v>3721.76</v>
+        <v>5221.63</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>13.55</v>
+        <v>7.3</v>
       </c>
       <c r="D14">
-        <v>17.37</v>
+        <v>33.44</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>309.36</v>
+        <v>175.35</v>
       </c>
       <c r="D15">
-        <v>326.25</v>
+        <v>710.01</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.7</v>
+        <v>0.44</v>
       </c>
       <c r="D16">
-        <v>1.2</v>
+        <v>5.96</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="D17">
-        <v>2.15</v>
+        <v>6.22</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="D18">
-        <v>0.96</v>
+        <v>6.04</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>11.74</v>
+        <v>5.9</v>
       </c>
       <c r="D19">
-        <v>16.52</v>
+        <v>41.81</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>4.06</v>
+        <v>1.54</v>
       </c>
       <c r="D20">
-        <v>5.76</v>
+        <v>32.38</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>3.74</v>
+        <v>6.48</v>
       </c>
       <c r="D21">
-        <v>51.94</v>
+        <v>86.90000000000001</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>41.23</v>
+        <v>481.54</v>
       </c>
       <c r="D22">
-        <v>661.71</v>
+        <v>10106.89</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>1.39</v>
+        <v>1.32</v>
       </c>
       <c r="D23">
-        <v>1.56</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>481.27</v>
+        <v>192.1</v>
       </c>
       <c r="D24">
-        <v>552.47</v>
+        <v>435.65</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>989.78</v>
+        <v>511.21</v>
       </c>
       <c r="D25">
-        <v>1406.34</v>
+        <v>2425.36</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>16.71</v>
+        <v>6.86</v>
       </c>
       <c r="D26">
-        <v>19.54</v>
+        <v>22.04</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#56 Use specific fitness calculation based on Nutrient signal
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -489,7 +489,7 @@
         <v>1307.95</v>
       </c>
       <c r="D2">
-        <v>4638.95</v>
+        <v>6141.95</v>
       </c>
       <c r="E2">
         <v>1765.61</v>
@@ -506,7 +506,7 @@
         <v>206.19</v>
       </c>
       <c r="D3">
-        <v>697.52</v>
+        <v>992.47</v>
       </c>
       <c r="E3">
         <v>971.0855</v>
@@ -523,7 +523,7 @@
         <v>42.31</v>
       </c>
       <c r="D4">
-        <v>162.59</v>
+        <v>179.42</v>
       </c>
       <c r="E4">
         <v>176.561</v>
@@ -540,7 +540,7 @@
         <v>40.18</v>
       </c>
       <c r="D5">
-        <v>144.5</v>
+        <v>182.88</v>
       </c>
       <c r="E5">
         <v>264.8415</v>
@@ -557,7 +557,7 @@
         <v>23.37</v>
       </c>
       <c r="D6">
-        <v>52.49</v>
+        <v>81.88</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -574,7 +574,7 @@
         <v>46.93</v>
       </c>
       <c r="D7">
-        <v>773.48</v>
+        <v>257.6</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -591,7 +591,7 @@
         <v>199.15</v>
       </c>
       <c r="D8">
-        <v>536.14</v>
+        <v>1379.76</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -608,7 +608,7 @@
         <v>0.75</v>
       </c>
       <c r="D9">
-        <v>1.17</v>
+        <v>3.2</v>
       </c>
       <c r="E9">
         <v>17.6561</v>
@@ -625,7 +625,7 @@
         <v>11.46</v>
       </c>
       <c r="D10">
-        <v>49.11</v>
+        <v>48.93</v>
       </c>
       <c r="E10">
         <v>176.561</v>
@@ -642,7 +642,7 @@
         <v>7.2</v>
       </c>
       <c r="D11">
-        <v>32.98</v>
+        <v>51.65</v>
       </c>
       <c r="E11">
         <v>105.9366</v>
@@ -659,7 +659,7 @@
         <v>1411.22</v>
       </c>
       <c r="D12">
-        <v>2808.04</v>
+        <v>5467.4</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -676,7 +676,7 @@
         <v>1418.91</v>
       </c>
       <c r="D13">
-        <v>5221.63</v>
+        <v>5674.82</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -693,7 +693,7 @@
         <v>7.3</v>
       </c>
       <c r="D14">
-        <v>33.44</v>
+        <v>27.5</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -710,7 +710,7 @@
         <v>175.35</v>
       </c>
       <c r="D15">
-        <v>710.01</v>
+        <v>751.48</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -727,7 +727,7 @@
         <v>0.44</v>
       </c>
       <c r="D16">
-        <v>5.96</v>
+        <v>1.99</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -744,7 +744,7 @@
         <v>0.99</v>
       </c>
       <c r="D17">
-        <v>6.22</v>
+        <v>1.65</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -761,7 +761,7 @@
         <v>0.54</v>
       </c>
       <c r="D18">
-        <v>6.04</v>
+        <v>2.34</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -778,7 +778,7 @@
         <v>5.9</v>
       </c>
       <c r="D19">
-        <v>41.81</v>
+        <v>29.44</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -795,7 +795,7 @@
         <v>1.54</v>
       </c>
       <c r="D20">
-        <v>32.38</v>
+        <v>4.59</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -812,7 +812,7 @@
         <v>6.48</v>
       </c>
       <c r="D21">
-        <v>86.90000000000001</v>
+        <v>75.26000000000001</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -829,7 +829,7 @@
         <v>481.54</v>
       </c>
       <c r="D22">
-        <v>10106.89</v>
+        <v>602.02</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -846,7 +846,7 @@
         <v>1.32</v>
       </c>
       <c r="D23">
-        <v>9.609999999999999</v>
+        <v>3.15</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -863,7 +863,7 @@
         <v>192.1</v>
       </c>
       <c r="D24">
-        <v>435.65</v>
+        <v>1289.85</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -880,7 +880,7 @@
         <v>511.21</v>
       </c>
       <c r="D25">
-        <v>2425.36</v>
+        <v>2413.84</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -897,7 +897,7 @@
         <v>6.86</v>
       </c>
       <c r="D26">
-        <v>22.04</v>
+        <v>31.69</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#65 Add function to select only adults
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1307.95</v>
+        <v>1404.55</v>
       </c>
       <c r="D2">
-        <v>6141.95</v>
+        <v>2999.55</v>
       </c>
       <c r="E2">
-        <v>1765.61</v>
+        <v>2989.87</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>206.19</v>
+        <v>194.79</v>
       </c>
       <c r="D3">
-        <v>992.47</v>
+        <v>510.09</v>
       </c>
       <c r="E3">
-        <v>971.0855</v>
+        <v>1644.4285</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>42.31</v>
+        <v>90.52</v>
       </c>
       <c r="D4">
-        <v>179.42</v>
+        <v>118.44</v>
       </c>
       <c r="E4">
-        <v>176.561</v>
+        <v>298.987</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>40.18</v>
+        <v>35.89</v>
       </c>
       <c r="D5">
-        <v>182.88</v>
+        <v>69.31999999999999</v>
       </c>
       <c r="E5">
-        <v>264.8415</v>
+        <v>448.4805000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>23.37</v>
+        <v>29.47</v>
       </c>
       <c r="D6">
-        <v>81.88</v>
+        <v>53.1</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>46.93</v>
+        <v>122.22</v>
       </c>
       <c r="D7">
-        <v>257.6</v>
+        <v>214.06</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>199.15</v>
+        <v>219.6</v>
       </c>
       <c r="D8">
-        <v>1379.76</v>
+        <v>1322.27</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="D9">
-        <v>3.2</v>
+        <v>2.16</v>
       </c>
       <c r="E9">
-        <v>17.6561</v>
+        <v>29.89870000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>11.46</v>
+        <v>11.01</v>
       </c>
       <c r="D10">
-        <v>48.93</v>
+        <v>25.14</v>
       </c>
       <c r="E10">
-        <v>176.561</v>
+        <v>298.987</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>7.2</v>
+        <v>11.47</v>
       </c>
       <c r="D11">
-        <v>51.65</v>
+        <v>16.5</v>
       </c>
       <c r="E11">
-        <v>105.9366</v>
+        <v>179.3922</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>1411.22</v>
+        <v>2623.22</v>
       </c>
       <c r="D12">
-        <v>5467.4</v>
+        <v>3053.74</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>1418.91</v>
+        <v>2241.43</v>
       </c>
       <c r="D13">
-        <v>5674.82</v>
+        <v>3804.86</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>7.3</v>
+        <v>13.55</v>
       </c>
       <c r="D14">
-        <v>27.5</v>
+        <v>16.64</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>175.35</v>
+        <v>309.36</v>
       </c>
       <c r="D15">
-        <v>751.48</v>
+        <v>532.41</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.44</v>
+        <v>0.7</v>
       </c>
       <c r="D16">
-        <v>1.99</v>
+        <v>1.16</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="D17">
-        <v>1.65</v>
+        <v>1.25</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="D18">
-        <v>2.34</v>
+        <v>0.97</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>5.9</v>
+        <v>11.74</v>
       </c>
       <c r="D19">
-        <v>29.44</v>
+        <v>15.53</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>1.54</v>
+        <v>4.06</v>
       </c>
       <c r="D20">
-        <v>4.59</v>
+        <v>1.82</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>6.48</v>
+        <v>3.74</v>
       </c>
       <c r="D21">
-        <v>75.26000000000001</v>
+        <v>56.88</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>481.54</v>
+        <v>41.23</v>
       </c>
       <c r="D22">
-        <v>602.02</v>
+        <v>401.67</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>1.32</v>
+        <v>1.39</v>
       </c>
       <c r="D23">
-        <v>3.15</v>
+        <v>1.85</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>192.1</v>
+        <v>481.27</v>
       </c>
       <c r="D24">
-        <v>1289.85</v>
+        <v>749.15</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>511.21</v>
+        <v>989.78</v>
       </c>
       <c r="D25">
-        <v>2413.84</v>
+        <v>1640.03</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>6.86</v>
+        <v>16.71</v>
       </c>
       <c r="D26">
-        <v>31.69</v>
+        <v>14.77</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#57 Integrate sodium intake targets into nutrition and fitness calculations.
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1404.55</v>
+        <v>2130.86</v>
       </c>
       <c r="D2">
-        <v>2999.55</v>
+        <v>2939.46</v>
       </c>
       <c r="E2">
-        <v>2989.87</v>
+        <v>2932.53</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>194.79</v>
+        <v>207.81</v>
       </c>
       <c r="D3">
-        <v>510.09</v>
+        <v>512.86</v>
       </c>
       <c r="E3">
-        <v>1644.4285</v>
+        <v>1612.8915</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>90.52</v>
+        <v>102.86</v>
       </c>
       <c r="D4">
-        <v>118.44</v>
+        <v>98.14</v>
       </c>
       <c r="E4">
-        <v>298.987</v>
+        <v>293.253</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>35.89</v>
+        <v>101.98</v>
       </c>
       <c r="D5">
-        <v>69.31999999999999</v>
+        <v>64.34999999999999</v>
       </c>
       <c r="E5">
-        <v>448.4805000000001</v>
+        <v>439.8795</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>29.47</v>
+        <v>14.08</v>
       </c>
       <c r="D6">
-        <v>53.1</v>
+        <v>42.25</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>122.22</v>
+        <v>373.54</v>
       </c>
       <c r="D7">
-        <v>214.06</v>
+        <v>272.53</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>219.6</v>
+        <v>776.75</v>
       </c>
       <c r="D8">
-        <v>1322.27</v>
+        <v>858.54</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.9</v>
+        <v>2.43</v>
       </c>
       <c r="D9">
-        <v>2.16</v>
+        <v>2.15</v>
       </c>
       <c r="E9">
-        <v>29.89870000000001</v>
+        <v>29.3253</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>11.01</v>
+        <v>41.02</v>
       </c>
       <c r="D10">
-        <v>25.14</v>
+        <v>19.54</v>
       </c>
       <c r="E10">
-        <v>298.987</v>
+        <v>293.253</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>11.47</v>
+        <v>21.37</v>
       </c>
       <c r="D11">
-        <v>16.5</v>
+        <v>20.08</v>
       </c>
       <c r="E11">
-        <v>179.3922</v>
+        <v>175.9518</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -656,13 +656,13 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2623.22</v>
+        <v>3454.54</v>
       </c>
       <c r="D12">
-        <v>3053.74</v>
+        <v>2196.35</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2241.43</v>
+        <v>1879.42</v>
       </c>
       <c r="D13">
-        <v>3804.86</v>
+        <v>4273.16</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>13.55</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>16.64</v>
+        <v>16.57</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>309.36</v>
+        <v>172.62</v>
       </c>
       <c r="D15">
-        <v>532.41</v>
+        <v>374.65</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.7</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D16">
-        <v>1.16</v>
+        <v>1.26</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.95</v>
+        <v>1.1</v>
       </c>
       <c r="D17">
-        <v>1.25</v>
+        <v>1.44</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.52</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D18">
-        <v>0.97</v>
+        <v>1.29</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>11.74</v>
+        <v>9.23</v>
       </c>
       <c r="D19">
-        <v>15.53</v>
+        <v>10.81</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>4.06</v>
+        <v>5.93</v>
       </c>
       <c r="D20">
-        <v>1.82</v>
+        <v>5.35</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>3.74</v>
+        <v>16.92</v>
       </c>
       <c r="D21">
-        <v>56.88</v>
+        <v>145.34</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>41.23</v>
+        <v>236.89</v>
       </c>
       <c r="D22">
-        <v>401.67</v>
+        <v>647.35</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>1.39</v>
+        <v>0.9</v>
       </c>
       <c r="D23">
-        <v>1.85</v>
+        <v>1.48</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>481.27</v>
+        <v>356.56</v>
       </c>
       <c r="D24">
-        <v>749.15</v>
+        <v>568.53</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>989.78</v>
+        <v>1262.93</v>
       </c>
       <c r="D25">
-        <v>1640.03</v>
+        <v>1416.36</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>16.71</v>
+        <v>18.83</v>
       </c>
       <c r="D26">
-        <v>14.77</v>
+        <v>19.15</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#69 Present the results as weight percentages for each specific nutrient.
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -489,7 +489,7 @@
         <v>2130.86</v>
       </c>
       <c r="D2">
-        <v>2939.46</v>
+        <v>2933.96</v>
       </c>
       <c r="E2">
         <v>2932.53</v>
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>207.81</v>
+        <v>7.086215656787824</v>
       </c>
       <c r="D3">
-        <v>512.86</v>
+        <v>7.086215656787824</v>
       </c>
       <c r="E3">
-        <v>1612.8915</v>
+        <v>7.086215656787824</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>102.86</v>
+        <v>3.507435559056514</v>
       </c>
       <c r="D4">
-        <v>98.14</v>
+        <v>3.507435559056514</v>
       </c>
       <c r="E4">
-        <v>293.253</v>
+        <v>3.507435559056514</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>101.98</v>
+        <v>3.47746826119426</v>
       </c>
       <c r="D5">
-        <v>64.34999999999999</v>
+        <v>3.47746826119426</v>
       </c>
       <c r="E5">
-        <v>439.8795</v>
+        <v>3.47746826119426</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -557,7 +557,7 @@
         <v>14.08</v>
       </c>
       <c r="D6">
-        <v>42.25</v>
+        <v>42.08</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -591,7 +591,7 @@
         <v>776.75</v>
       </c>
       <c r="D8">
-        <v>858.54</v>
+        <v>856.46</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>2.43</v>
+        <v>0.0828772425175531</v>
       </c>
       <c r="D9">
-        <v>2.15</v>
+        <v>0.0828772425175531</v>
       </c>
       <c r="E9">
-        <v>29.3253</v>
+        <v>0.0828772425175531</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>41.02</v>
+        <v>1.398935390260287</v>
       </c>
       <c r="D10">
-        <v>19.54</v>
+        <v>1.398935390260287</v>
       </c>
       <c r="E10">
-        <v>293.253</v>
+        <v>1.398935390260287</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>21.37</v>
+        <v>0.7288041384060862</v>
       </c>
       <c r="D11">
-        <v>20.08</v>
+        <v>0.7288041384060862</v>
       </c>
       <c r="E11">
-        <v>175.9518</v>
+        <v>0.7288041384060862</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -659,7 +659,7 @@
         <v>3454.54</v>
       </c>
       <c r="D12">
-        <v>2196.35</v>
+        <v>2194.78</v>
       </c>
       <c r="E12">
         <v>2000</v>
@@ -676,7 +676,7 @@
         <v>1879.42</v>
       </c>
       <c r="D13">
-        <v>4273.16</v>
+        <v>4242.02</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -693,7 +693,7 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>16.57</v>
+        <v>16.54</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -710,7 +710,7 @@
         <v>172.62</v>
       </c>
       <c r="D15">
-        <v>374.65</v>
+        <v>372.69</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -727,7 +727,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="D16">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -744,7 +744,7 @@
         <v>1.1</v>
       </c>
       <c r="D17">
-        <v>1.44</v>
+        <v>1.43</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -761,7 +761,7 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="D18">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -812,7 +812,7 @@
         <v>16.92</v>
       </c>
       <c r="D21">
-        <v>145.34</v>
+        <v>144.65</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -846,7 +846,7 @@
         <v>0.9</v>
       </c>
       <c r="D23">
-        <v>1.48</v>
+        <v>1.46</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -880,7 +880,7 @@
         <v>1262.93</v>
       </c>
       <c r="D25">
-        <v>1416.36</v>
+        <v>1414.87</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -897,7 +897,7 @@
         <v>18.83</v>
       </c>
       <c r="D26">
-        <v>19.15</v>
+        <v>19.13</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#68 Change mealCode to V9001
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2130.86</v>
+        <v>2552.85</v>
       </c>
       <c r="D2">
-        <v>2933.96</v>
+        <v>3055.85</v>
       </c>
       <c r="E2">
-        <v>2932.53</v>
+        <v>3056.66</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,13 +503,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>7.086215656787824</v>
+        <v>13.14009408962724</v>
       </c>
       <c r="D3">
-        <v>7.086215656787824</v>
+        <v>15.25285769434612</v>
       </c>
       <c r="E3">
-        <v>7.086215656787824</v>
+        <v>55.00000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -520,13 +520,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3.507435559056514</v>
+        <v>2.985055583545438</v>
       </c>
       <c r="D4">
-        <v>3.507435559056514</v>
+        <v>3.705122584782082</v>
       </c>
       <c r="E4">
-        <v>3.507435559056514</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>3.47746826119426</v>
+        <v>2.466577898752233</v>
       </c>
       <c r="D5">
-        <v>3.47746826119426</v>
+        <v>3.059218231664627</v>
       </c>
       <c r="E5">
-        <v>3.47746826119426</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>14.08</v>
+        <v>48.82</v>
       </c>
       <c r="D6">
-        <v>42.08</v>
+        <v>56.86</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>373.54</v>
+        <v>414.26</v>
       </c>
       <c r="D7">
-        <v>272.53</v>
+        <v>472.09</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>776.75</v>
+        <v>312.69</v>
       </c>
       <c r="D8">
-        <v>856.46</v>
+        <v>929.72</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.0828772425175531</v>
+        <v>0.09551274920992193</v>
       </c>
       <c r="D9">
-        <v>0.0828772425175531</v>
+        <v>0.1121976274757415</v>
       </c>
       <c r="E9">
-        <v>0.0828772425175531</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.398935390260287</v>
+        <v>0.6831737910006347</v>
       </c>
       <c r="D10">
-        <v>1.398935390260287</v>
+        <v>1.023087291357233</v>
       </c>
       <c r="E10">
-        <v>1.398935390260287</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.7288041384060862</v>
+        <v>0.8145066837659403</v>
       </c>
       <c r="D11">
-        <v>0.7288041384060862</v>
+        <v>0.8375710743098677</v>
       </c>
       <c r="E11">
-        <v>0.7288041384060862</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>3454.54</v>
+        <v>4516.96</v>
       </c>
       <c r="D12">
-        <v>2194.78</v>
+        <v>5120.24</v>
       </c>
       <c r="E12">
         <v>2000</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>1879.42</v>
+        <v>2689.67</v>
       </c>
       <c r="D13">
-        <v>4242.02</v>
+        <v>4021.14</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>15</v>
+        <v>23.85</v>
       </c>
       <c r="D14">
-        <v>16.54</v>
+        <v>25.49</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>172.62</v>
+        <v>418.41</v>
       </c>
       <c r="D15">
-        <v>372.69</v>
+        <v>529.59</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.6899999999999999</v>
+        <v>1.53</v>
       </c>
       <c r="D16">
-        <v>1.25</v>
+        <v>2.24</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>1.1</v>
+        <v>2.45</v>
       </c>
       <c r="D17">
-        <v>1.43</v>
+        <v>3.1</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.6899999999999999</v>
+        <v>1.86</v>
       </c>
       <c r="D18">
-        <v>1.28</v>
+        <v>1.94</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>9.23</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="D19">
-        <v>10.81</v>
+        <v>11.59</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>5.93</v>
+        <v>3.33</v>
       </c>
       <c r="D20">
-        <v>5.35</v>
+        <v>4.97</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>16.92</v>
+        <v>13.72</v>
       </c>
       <c r="D21">
-        <v>144.65</v>
+        <v>72.23999999999999</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>236.89</v>
+        <v>81.92</v>
       </c>
       <c r="D22">
-        <v>647.35</v>
+        <v>700.29</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.9</v>
+        <v>1.95</v>
       </c>
       <c r="D23">
-        <v>1.46</v>
+        <v>2.38</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>356.56</v>
+        <v>1003.95</v>
       </c>
       <c r="D24">
-        <v>568.53</v>
+        <v>1087.97</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>1262.93</v>
+        <v>1214.07</v>
       </c>
       <c r="D25">
-        <v>1414.87</v>
+        <v>1670.54</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>18.83</v>
+        <v>12.53</v>
       </c>
       <c r="D26">
-        <v>19.13</v>
+        <v>15.4</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#74 Change base CONSUMO file to the original
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2552.85</v>
+        <v>1728.68</v>
       </c>
       <c r="D2">
-        <v>3055.85</v>
+        <v>2453.18</v>
       </c>
       <c r="E2">
-        <v>3056.66</v>
+        <v>1971.59</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,10 +503,10 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>13.14009408962724</v>
+        <v>9.046794718983156</v>
       </c>
       <c r="D3">
-        <v>15.25285769434612</v>
+        <v>17.54551909879843</v>
       </c>
       <c r="E3">
         <v>55.00000000000001</v>
@@ -520,10 +520,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>2.985055583545438</v>
+        <v>3.390603523044852</v>
       </c>
       <c r="D4">
-        <v>3.705122584782082</v>
+        <v>4.001278156208947</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -537,10 +537,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>2.466577898752233</v>
+        <v>4.360764662024051</v>
       </c>
       <c r="D5">
-        <v>3.059218231664627</v>
+        <v>4.396522603583909</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>48.82</v>
+        <v>11.7</v>
       </c>
       <c r="D6">
-        <v>56.86</v>
+        <v>31.45</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>414.26</v>
+        <v>198.39</v>
       </c>
       <c r="D7">
-        <v>472.09</v>
+        <v>195.3</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>312.69</v>
+        <v>763.84</v>
       </c>
       <c r="D8">
-        <v>929.72</v>
+        <v>997.88</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,10 +605,10 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.09551274920992193</v>
+        <v>0.192012538103764</v>
       </c>
       <c r="D9">
-        <v>0.1121976274757415</v>
+        <v>0.2034246471122292</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -622,10 +622,10 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0.6831737910006347</v>
+        <v>1.300402213441943</v>
       </c>
       <c r="D10">
-        <v>1.023087291357233</v>
+        <v>1.324748045993335</v>
       </c>
       <c r="E10">
         <v>10</v>
@@ -639,10 +639,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.8145066837659403</v>
+        <v>0.9168336215947533</v>
       </c>
       <c r="D11">
-        <v>0.8375710743098677</v>
+        <v>0.9300209475600909</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>4516.96</v>
+        <v>2481.08</v>
       </c>
       <c r="D12">
-        <v>5120.24</v>
+        <v>2489.84</v>
       </c>
       <c r="E12">
         <v>2000</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>2689.67</v>
+        <v>1610.56</v>
       </c>
       <c r="D13">
-        <v>4021.14</v>
+        <v>3931.56</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>23.85</v>
+        <v>10.52</v>
       </c>
       <c r="D14">
-        <v>25.49</v>
+        <v>14.92</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>418.41</v>
+        <v>147.54</v>
       </c>
       <c r="D15">
-        <v>529.59</v>
+        <v>303.81</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>1.53</v>
+        <v>0.75</v>
       </c>
       <c r="D16">
-        <v>2.24</v>
+        <v>1.4</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>2.45</v>
+        <v>0.68</v>
       </c>
       <c r="D17">
-        <v>3.1</v>
+        <v>1.12</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>1.86</v>
+        <v>0.39</v>
       </c>
       <c r="D18">
-        <v>1.94</v>
+        <v>1.15</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>9.460000000000001</v>
+        <v>5.52</v>
       </c>
       <c r="D19">
-        <v>11.59</v>
+        <v>12.77</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>3.33</v>
+        <v>3.96</v>
       </c>
       <c r="D20">
-        <v>4.97</v>
+        <v>3.87</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>13.72</v>
+        <v>122.35</v>
       </c>
       <c r="D21">
-        <v>72.23999999999999</v>
+        <v>189.97</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>81.92</v>
+        <v>224.21</v>
       </c>
       <c r="D22">
-        <v>700.29</v>
+        <v>759.46</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>1.95</v>
+        <v>0.74</v>
       </c>
       <c r="D23">
-        <v>2.38</v>
+        <v>1.07</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>1003.95</v>
+        <v>300.69</v>
       </c>
       <c r="D24">
-        <v>1087.97</v>
+        <v>508.49</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>1214.07</v>
+        <v>972.77</v>
       </c>
       <c r="D25">
-        <v>1670.54</v>
+        <v>1244.86</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>12.53</v>
+        <v>11.57</v>
       </c>
       <c r="D26">
-        <v>15.4</v>
+        <v>13.4</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#74 Update CHOTOT, PTN, and LIP levels to use kcal instead of grams.
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -486,13 +486,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1728.68</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>2453.18</v>
+        <v>2438.75</v>
       </c>
       <c r="E2">
-        <v>1971.59</v>
+        <v>2388.84</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -503,10 +503,10 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>9.046794718983156</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>17.54551909879843</v>
+        <v>83.66068886991174</v>
       </c>
       <c r="E3">
         <v>55.00000000000001</v>
@@ -520,10 +520,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>3.390603523044852</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>4.001278156208947</v>
+        <v>11.25441636945128</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -537,13 +537,13 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>4.360764662024051</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>4.396522603583909</v>
+        <v>4.529395020177157</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -554,10 +554,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>11.7</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>31.45</v>
+        <v>35.64</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -571,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>198.39</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>195.3</v>
+        <v>238.83</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -588,10 +588,10 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>763.84</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>997.88</v>
+        <v>879.5599999999999</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -605,13 +605,13 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0.192012538103764</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.2034246471122292</v>
+        <v>0.189213174595201</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -622,13 +622,13 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>1.300402213441943</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1.324748045993335</v>
+        <v>2.468562147318364</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>4.444444444444445</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -639,13 +639,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.9168336215947533</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.9300209475600909</v>
+        <v>0.5270340416268984</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -656,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>2481.08</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>2489.84</v>
+        <v>1534.53</v>
       </c>
       <c r="E12">
         <v>2000</v>
@@ -673,10 +673,10 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>1610.56</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>3931.56</v>
+        <v>3569.46</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -690,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>10.52</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>14.92</v>
+        <v>14.42</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -707,10 +707,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>147.54</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>303.81</v>
+        <v>312.5</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1.4</v>
+        <v>1.56</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C17">
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1.12</v>
+        <v>2.45</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -758,10 +758,10 @@
         <v>20</v>
       </c>
       <c r="C18">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1.15</v>
+        <v>1.11</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -775,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="C19">
-        <v>5.52</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>12.77</v>
+        <v>11.8</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -792,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>3.96</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>3.87</v>
+        <v>18.67</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -809,10 +809,10 @@
         <v>23</v>
       </c>
       <c r="C21">
-        <v>122.35</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>189.97</v>
+        <v>68.26000000000001</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -826,10 +826,10 @@
         <v>24</v>
       </c>
       <c r="C22">
-        <v>224.21</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>759.46</v>
+        <v>3519.75</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -843,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>1.07</v>
+        <v>4.16</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>300.69</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>508.49</v>
+        <v>449.36</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -877,10 +877,10 @@
         <v>27</v>
       </c>
       <c r="C25">
-        <v>972.77</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1244.86</v>
+        <v>1058.93</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -894,10 +894,10 @@
         <v>28</v>
       </c>
       <c r="C26">
-        <v>11.57</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>13.4</v>
+        <v>9.6</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>

<commit_message>
#75 Create a function to generate a polar graph to show the results
</commit_message>
<xml_diff>
--- a/notebooks/samples/output/test_result.xlsx
+++ b/notebooks/samples/output/test_result.xlsx
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2438.75</v>
+        <v>2119.75</v>
       </c>
       <c r="E2">
         <v>2388.84</v>
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>83.66068886991174</v>
+        <v>62.98161450745967</v>
       </c>
       <c r="E3">
         <v>55.00000000000001</v>
@@ -523,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>11.25441636945128</v>
+        <v>13.78116575408985</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>4.529395020177157</v>
+        <v>6.383432963279248</v>
       </c>
       <c r="E5">
         <v>6.666666666666667</v>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>35.64</v>
+        <v>32.1</v>
       </c>
       <c r="E6">
         <v>31</v>
@@ -574,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>238.83</v>
+        <v>178.25</v>
       </c>
       <c r="E7">
         <v>300</v>
@@ -591,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>879.5599999999999</v>
+        <v>888.66</v>
       </c>
       <c r="E8">
         <v>868</v>
@@ -608,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0.189213174595201</v>
+        <v>0.2461445722610137</v>
       </c>
       <c r="E9">
         <v>0.4444444444444444</v>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>2.468562147318364</v>
+        <v>2.982200565965071</v>
       </c>
       <c r="E10">
         <v>4.444444444444445</v>
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>0.5270340416268984</v>
+        <v>0.8317844644262485</v>
       </c>
       <c r="E11">
         <v>2.666666666666667</v>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1534.53</v>
+        <v>2857.59</v>
       </c>
       <c r="E12">
         <v>2000</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3569.46</v>
+        <v>3510.83</v>
       </c>
       <c r="E13">
         <v>3510</v>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>14.42</v>
+        <v>15.4</v>
       </c>
       <c r="E14">
         <v>6.8</v>
@@ -710,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>312.5</v>
+        <v>305.16</v>
       </c>
       <c r="E15">
         <v>303</v>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="E16">
         <v>0.9</v>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>2.45</v>
+        <v>1.96</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1.11</v>
+        <v>1.31</v>
       </c>
       <c r="E18">
         <v>1.1</v>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>11.8</v>
+        <v>15.94</v>
       </c>
       <c r="E19">
         <v>11.5</v>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>18.67</v>
+        <v>3.74</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -812,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>68.26000000000001</v>
+        <v>66.2</v>
       </c>
       <c r="E21">
         <v>66.09999999999999</v>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>3519.75</v>
+        <v>1057.74</v>
       </c>
       <c r="E22">
         <v>560</v>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>4.16</v>
+        <v>1.29</v>
       </c>
       <c r="E23">
         <v>0.7</v>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>449.36</v>
+        <v>667.76</v>
       </c>
       <c r="E24">
         <v>322</v>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1058.93</v>
+        <v>1180.86</v>
       </c>
       <c r="E25">
         <v>649</v>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>9.6</v>
+        <v>10.75</v>
       </c>
       <c r="E26">
         <v>8</v>

</xml_diff>